<commit_message>
Added Convolution Figure Results
</commit_message>
<xml_diff>
--- a/All Session Data and Results/Raw Session Data Sheets/32-Minute Sessions/NS016/27-Sep-2023_NS016_Go-No-Go_Session#39.xlsx
+++ b/All Session Data and Results/Raw Session Data Sheets/32-Minute Sessions/NS016/27-Sep-2023_NS016_Go-No-Go_Session#39.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Current Projects and Data\Stimulation Project\Behavior Data\New Paradigm Data\ExcelSessionData\SessionDataSheets\NS016\Go-No-Go\Week 15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\ArucoDetection\All Session Data and Results\Raw Session Data Sheets\32-Minute Sessions\NS016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1533F4-5FA3-4A63-A4B6-018866BC3311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EEB2E9-33BE-42F9-B6A7-073852A96D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{3F6160D7-DA1A-4C2E-856A-1DCB1F0E59BE}"/>
+    <workbookView xWindow="22932" yWindow="-4764" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{3F6160D7-DA1A-4C2E-856A-1DCB1F0E59BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,10 +240,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +630,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:X2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E231E91D-F7A2-4168-ADCA-2B7CD8F8910C}">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1048576"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5846,1161 +5847,1073 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B527612D-EFD2-4156-9454-24BCA623320A}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1.0006166666667318</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>8.4000000002561137E-2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>0.15975000000010672</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
         <v>3.4214166666667247</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>8.2000000002153683E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>1.2476666666666765</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>9.1999999996914994E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.32921666666673749</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
         <v>3.9375166666667307</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>1.4970333333333352</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>9.4999999993888196E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.49966666666672005</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
         <v>4.1005000000001015</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.1860000000015134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>1.9165666666667676</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>9.5000000001164153E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.67118333333334401</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
         <v>4.5811166666667607</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2.1682333333334101</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.18699999999807915</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>0.840383333333375</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
         <v>4.8379666666667616</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>2.5828333333333529</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>7.4999999997089617E-2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1.756666666666691</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
         <v>5.494550000000042</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.34100000000034925</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>2.8307833333333594</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>9.30000000007567E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>2.4236833333333681</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
         <v>6.1752833333334518</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>4.9984333333333781</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>9.1999999996914994E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>3.0903833333333752</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
         <v>6.3412500000000973</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>0.59200000000419095</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>5.2470000000001162</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>0.18800000000192085</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>3.2599000000000768</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
         <v>6.8405000000000049</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>7.0011666666667827</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>9.2000000004190952E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>3.6784666666667665</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
         <v>7.6632833333334327</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>9.4000000004598405E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>7.2511333333334429</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>0.27800000000570435</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>5.7431333333333896</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
         <v>8.5991333333334001</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>8.0894833333334351</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>0.45300000000133878</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>5.9139000000000426</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
         <v>8.7666666666666675</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>0.60499999999592546</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>9.0163666666667268</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>1.1679999999978463</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>6.5827000000001137</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
         <v>9.4964833333334049</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>11.43068333333334</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>9.2999999993480742E-2</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>7.5032500000001168</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
         <v>10.013050000000051</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>0.98099999999976717</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>11.680583333333439</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>9.30000000007567E-2</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>7.9222166666667668</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
         <v>10.840450000000056</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>11.938550000000031</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>0.57800000000133878</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>8.336716666666689</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
         <v>11.101333333333363</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>12.352183333333354</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>0.71699999999691499</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>9.2383500000001124</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
         <v>12.584650000000087</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>0.37099999999918509</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>13.008050000000003</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>0.97299999999813735</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>9.6665333333334278</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
         <v>13.328200000000045</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>13.910150000000067</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>0.27799999999842839</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>9.8361666666667595</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
         <v>13.492233333333449</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>0.26200000000244472</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>14.158966666666675</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>0.54399999999441206</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>10.243000000000029</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
         <v>14.492383333333418</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>15.523700000000099</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>0.45100000000093132</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>10.413666666666783</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
         <v>14.653966666666747</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>8.2000000002153683E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>15.790800000000067</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>1.9340000000011059</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>10.582000000000091</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
         <v>15.188416666666672</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>15.997300000000056</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>1.2240000000019791</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>11.270266666666673</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
         <v>16.551450000000113</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>16.214366666666685</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>0.4680000000007567</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>12.180000000000048</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
         <v>16.713500000000082</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>9.5999999997729901E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>17.398083333333368</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>0.36200000000098953</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>12.833650000000004</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
         <v>17.06305000000005</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>17.986700000000081</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>0.61299999999755528</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>13.745083333333362</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
         <v>18.220450000000103</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>0.18800000000192085</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>18.635850000000087</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>0.17399999999906868</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>14.91263333333336</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
         <v>18.981700000000032</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>19.146600000000035</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>9.3999999997322448E-2</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>15.357883333333424</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
         <v>19.395733333333435</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>9.30000000007567E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>20.010050000000046</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
         <v>17.231833333333391</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
         <v>19.746550000000084</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>20.850716666666752</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>0.36300000000483124</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>17.647066666666674</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
         <v>20.351250000000071</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>0.63599999999860302</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>22.106883333333339</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>0.35800000000017462</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>17.816766666666688</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
         <v>20.682750000000063</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>22.62498333333339</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>1.1019999999989523</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>18.473883333333408</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
         <v>21.529183333333396</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>23.914866666666786</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>1.4639999999999418</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <v>20.180100000000071</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
         <v>21.872916666666665</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>0.76299999999901047</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>24.126433333333384</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>0.45300000000133878</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="3">
         <v>21.100716666666752</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
         <v>22.446783333333347</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>26.233266666666776</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>0.26499999999941792</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <v>21.269266666666713</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
         <v>22.888833333333363</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>2.8849999999947613</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>27.498266666666677</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>0.61999999999534339</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <v>21.699266666666759</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
         <v>23.084933333333417</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <v>1.4040000000022701</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>27.730833333333429</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>9.4000000004598405E-2</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <v>23.300683333333414</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
         <v>23.560800000000018</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>28.763416666666672</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>0.34099999999307329</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>23.730450000000079</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
         <v>24.367833333333451</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <v>9.5000000001164153E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>30.783500000000036</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>8.6999999999534339E-2</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>24.625266666666722</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
         <v>24.888100000000001</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>32.014533333333382</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>1.1010000000023865</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <v>26.065683333333435</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
         <v>25.150133333333361</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>13.514783333333252</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3">
         <v>26.736816666666709</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
         <v>25.332150000000063</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <v>1.2240000000019791</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>13.772833333333256</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3">
         <v>26.906266666666731</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
         <v>25.545683333333365</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>7.8999999997904524E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>14.029666666666648</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3">
         <v>27.328450000000036</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
         <v>25.896800000000077</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>14.627433333333345</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3">
         <v>29.526716666666712</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
         <v>26.477666666666725</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>9.1999999996914994E-2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>15.565116666666654</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>14.966883333333318</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3">
         <v>27.069783333333422</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>8.0999999998311978E-2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>16.671316666666584</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>15.136449999999968</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3">
         <v>28.079816666666737</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>16.832599999999971</v>
-      </c>
-      <c r="B48">
-        <v>0.22400000000197906</v>
-      </c>
-      <c r="C48">
-        <v>15.306866666666611</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
         <v>28.340650000000096</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>17.438816666666632</v>
-      </c>
-      <c r="B49">
-        <v>1.3929999999963911</v>
-      </c>
-      <c r="C49">
-        <v>15.735633333333316</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3">
         <v>28.508050000000004</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>9.5999999997729901E-2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>17.809733333333256</v>
-      </c>
-      <c r="B50">
-        <v>2.113999999994121</v>
-      </c>
-      <c r="C50">
-        <v>15.903449999999914</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3">
         <v>29.10640000000009</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>18.304416666666658</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>16.072966666666616</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3">
         <v>29.2695166666667</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>9.1999999996914994E-2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>18.73189999999995</v>
-      </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <v>16.241800000000026</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3">
         <v>29.787833333333403</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>18.992633333333288</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>16.411616666666667</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3">
         <v>30.047400000000078</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>19.327283333333252</v>
-      </c>
-      <c r="B54">
-        <v>0.3129999999946449</v>
-      </c>
-      <c r="C54">
-        <v>17.087799999999941</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3">
         <v>30.261300000000119</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>3.2080000000059954</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C55">
-        <v>17.258349999999943</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3">
         <v>30.546166666666736</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>0.44400000000314321</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C56">
-        <v>18.041999999999948</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3">
         <v>31.051033333333422</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>1.0260000000052969</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C57">
-        <v>18.472999999999956</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3">
         <v>31.310416666666665</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <v>2.3699999999953434</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C58">
-        <v>19.16343333333328</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3">
         <v>31.587550000000071</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E59">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3">
         <v>31.75605000000008</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <v>0.375</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E60">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3">
         <v>32.32988333333342</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7013,7 +6926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107FFE73-E444-404C-BC8A-07322648C0BF}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -7874,7 +7787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDDA2A9-141D-4461-9310-EFC4942A2F6B}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -9090,7 +9003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1177233E-7EEC-4C7D-AA6C-0DFC57E8E5D1}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
@@ -9351,6 +9264,1554 @@
       </c>
       <c r="F13" s="2" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>22</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>23</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>18</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>20</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>27</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>22</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>28</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>23</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>25</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>29</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>30</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>31</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>32</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>27</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>29</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>29</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>33</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>31</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>34</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>35</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>32</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>36</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>34</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>37</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>37</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>38</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>39</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>39</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>40</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>43</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>40</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>41</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>42</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>43</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>46</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>47</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>49</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>44</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>51</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>52</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>57</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>59</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="M">
+      <formula>NOT(ISERROR(SEARCH("M",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FA">
+      <formula>NOT(ISERROR(SEARCH("FA",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B5442F-FCC3-4F12-8CE9-58627A06FB4B}">
+  <dimension ref="A1:F76"/>
+  <sheetViews>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -10632,1552 +12093,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B5442F-FCC3-4F12-8CE9-58627A06FB4B}">
-  <dimension ref="A1:F76"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>11</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>7</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>9</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>14</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>15</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>16</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>11</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>17</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>13</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>18</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>19</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>20</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>21</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>0</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>22</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>15</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>0</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>16</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>23</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>0</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>24</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>0</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>25</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>0</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>18</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>26</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>0</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>20</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>27</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>0</v>
-      </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>22</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>0</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>28</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>2</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>23</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>0</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>25</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>0</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>29</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>0</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>30</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>0</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>31</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>0</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>32</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>0</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>27</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>29</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>0</v>
-      </c>
-      <c r="B50">
-        <v>29</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>0</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>33</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>0</v>
-      </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52">
-        <v>31</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>0</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>34</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>0</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>35</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>0</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>32</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>0</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>36</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>0</v>
-      </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>34</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>0</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>37</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>0</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59">
-        <v>37</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>0</v>
-      </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-      <c r="C60">
-        <v>38</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>0</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>39</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>0</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>39</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>0</v>
-      </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>40</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>0</v>
-      </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>43</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>0</v>
-      </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
-      <c r="C65">
-        <v>40</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>0</v>
-      </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>41</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>0</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67">
-        <v>42</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>0</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>43</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>0</v>
-      </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <v>46</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>0</v>
-      </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-      <c r="D70">
-        <v>47</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>0</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>49</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>0</v>
-      </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72">
-        <v>44</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>0</v>
-      </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73">
-        <v>51</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>0</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <v>52</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>0</v>
-      </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75">
-        <v>57</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>0</v>
-      </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>59</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="M">
-      <formula>NOT(ISERROR(SEARCH("M",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FA">
-      <formula>NOT(ISERROR(SEARCH("FA",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>